<commit_message>
Google Sheet converted to .csv, .xlsx, and .ttl files
</commit_message>
<xml_diff>
--- a/vocabularies/vocabulary.xlsx
+++ b/vocabularies/vocabulary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L164"/>
+  <dimension ref="A1:M165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,7 @@
       <c r="J1" t="inlineStr"/>
       <c r="K1" t="inlineStr"/>
       <c r="L1" t="inlineStr"/>
+      <c r="M1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -464,6 +465,7 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -494,6 +496,7 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -524,6 +527,7 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -554,6 +558,7 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -584,15 +589,24 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Metadata about vocabulary</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
+          <t>PREFIX</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>rtd</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://datacite-metadata-schema.readthedocs.io/en/4.5/</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -602,23 +616,16 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>dct:title</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>DataCite Controlled Terms</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Title of the vocabulary</t>
-        </is>
-      </c>
+          <t>Metadata about vocabulary</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
@@ -628,21 +635,22 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>dct:description</t>
+          <t>dct:title</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Controlled vocabulary of terms used in Datacite Schema 4.5</t>
+          <t>DataCite Controlled Terms</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Description of the controlled vocabulary</t>
+          <t>Title of the vocabulary</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -654,21 +662,22 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dct:contributor</t>
+          <t>dct:description</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://orcid.org/0000-0002-9381-9693</t>
+          <t>Controlled vocabulary of terms used in Datacite Schema 4.5</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>An ORCID ID of the vocabulary creator, repeat this row as needed.</t>
+          <t>Description of the controlled vocabulary</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -680,21 +689,22 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dct:rights</t>
+          <t>dct:contributor</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://spdx.org/licenses/CC0-1.0</t>
+          <t>https://orcid.org/0000-0002-9381-9693</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>License under which the vocabulary is provided</t>
+          <t>An ORCID ID of the vocabulary creator, repeat this row as needed.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -706,21 +716,22 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>pav:version</t>
+          <t>dct:rights</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4.5.0</t>
+          <t>https://spdx.org/licenses/CC0-1.0</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Vocabulary version</t>
+          <t>License under which the vocabulary is provided</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -732,21 +743,22 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>pav:createdOn</t>
+          <t>pav:version</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2022-05-03T12:00+02:00</t>
+          <t>4.5.0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Date when vocabulary was initially created</t>
+          <t>Vocabulary version</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -758,11 +770,12 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>pav:lastUpdatedOn</t>
+          <t>pav:createdOn</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -772,7 +785,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Date of the last vocabulary update</t>
+          <t>Date when vocabulary was initially created</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -784,15 +797,24 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Definition of terms</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+          <t>pav:lastUpdatedOn</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2022-05-03T12:00+02:00</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Date of the last vocabulary update</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
@@ -802,135 +824,135 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Identifier</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>skos:prefLabel@en</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>skos:definition@en</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>skos:altLabel(separator=",")</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>dct:source(separator=",")</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>skos:broader(separator=",")</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>skos:exactMatch(separator=",")</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>skos:closeMatch(separator=",")</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>skos:editorialNote@en</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>dct:creator(separator=",")</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>dct:contributor(separator=",")</t>
-        </is>
-      </c>
+          <t>Definition of terms</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>datacite:resourceTypeGeneral</t>
+          <t>Identifier</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>resourceTypeGeneral</t>
+          <t>skos:prefLabel@en</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>The general type of a resource.</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
+          <t>skos:definition@en</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>skos:altLabel(separator=",")</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>dct:source(separator=",")</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>skos:broader(separator=",")</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>skos:exactMatch(separator=",")</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>skos:closeMatch(separator=",")</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>skos:editorialNote@en</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>dct:creator(separator=",")</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>dct:contributor(separator=",")</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>purl_target</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>datacite:Audiovisual</t>
+          <t>datacite:resourceTypeGeneral</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Audiovisual</t>
+          <t>resourceTypeGeneral</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>A series of visual representations imparting an impression of motion when shown in succession. May or may not include sound.</t>
+          <t>The general type of a resource.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>datacite:resourceTypeGeneral</t>
-        </is>
-      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>rtd:appendix-1/resourceTypeGeneral/</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>datacite:Book</t>
+          <t>datacite:Audiovisual</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Book</t>
+          <t>Audiovisual</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>A medium for recording information in the form of writing or images, typically composed of many pages bound together and protected by a cover.</t>
+          <t>A series of visual representations imparting an impression of motion when shown in succession. May or may not include sound.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -946,21 +968,22 @@
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>datacite:BookChapter</t>
+          <t>datacite:Book</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BookChapter</t>
+          <t>Book</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>One of the main divisions of a book.</t>
+          <t>A medium for recording information in the form of writing or images, typically composed of many pages bound together and protected by a cover.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -976,21 +999,22 @@
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>datacite:Collection</t>
+          <t>datacite:BookChapter</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Collection</t>
+          <t>BookChapter</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>An aggregation of resources, which may encompass collections of one resourceType as well as those of mixed types. A collection is described as a group; its parts may also be separately described.</t>
+          <t>One of the main divisions of a book.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -1006,21 +1030,22 @@
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>datacite:ComputationalNotebook</t>
+          <t>datacite:Collection</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ComputationalNotebook</t>
+          <t>Collection</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>A virtual notebook environment used for literate programming.</t>
+          <t>An aggregation of resources, which may encompass collections of one resourceType as well as those of mixed types. A collection is described as a group; its parts may also be separately described.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -1036,21 +1061,22 @@
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>datacite:ConferencePaper</t>
+          <t>datacite:ComputationalNotebook</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ConferencePaper</t>
+          <t>ComputationalNotebook</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Article that is written with the goal of being accepted to a conference.</t>
+          <t>A virtual notebook environment used for literate programming.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
@@ -1066,21 +1092,22 @@
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>datacite:ConferenceProceeding</t>
+          <t>datacite:ConferencePaper</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ConferenceProceeding</t>
+          <t>ConferencePaper</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Collection of academic papers published in the context of an academic conference.</t>
+          <t>Article that is written with the goal of being accepted to a conference.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -1096,21 +1123,22 @@
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>datacite:DataPaper</t>
+          <t>datacite:ConferenceProceeding</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>DataPaper</t>
+          <t>ConferenceProceeding</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>A factual and objective publication with a focused intent to identify and describe specific data, sets of data, or data collections to facilitate discoverability.</t>
+          <t>Collection of academic papers published in the context of an academic conference.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -1126,21 +1154,22 @@
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>datacite:Dataset</t>
+          <t>datacite:DataPaper</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Dataset</t>
+          <t>DataPaper</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Data encoded in a defined structure.</t>
+          <t>A factual and objective publication with a focused intent to identify and describe specific data, sets of data, or data collections to facilitate discoverability.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -1156,21 +1185,22 @@
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>datacite:Dissertation</t>
+          <t>datacite:Dataset</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Dissertation</t>
+          <t>Dataset</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>A written essay, treatise, or thesis, especially one written by a candidate for the degree of Doctor of Philosophy.</t>
+          <t>Data encoded in a defined structure.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -1186,21 +1216,22 @@
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>datacite:Event</t>
+          <t>datacite:Dissertation</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Event</t>
+          <t>Dissertation</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>A non-persistent, time-based occurrence.</t>
+          <t>A written essay, treatise, or thesis, especially one written by a candidate for the degree of Doctor of Philosophy.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -1216,21 +1247,22 @@
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>datacite:Image</t>
+          <t>datacite:Event</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Image</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>A visual representation other than text.</t>
+          <t>A non-persistent, time-based occurrence.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -1246,21 +1278,22 @@
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>datacite:Instrument</t>
+          <t>datacite:Image</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Instrument</t>
+          <t>Image</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>A device, tool or apparatus used to obtain, measure and/or analyze data.</t>
+          <t>A visual representation other than text.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -1276,21 +1309,22 @@
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>datacite:InteractiveResource</t>
+          <t>datacite:Instrument</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>InteractiveResource</t>
+          <t>Instrument</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>A resource requiring interaction from the user to be understood, executed, or experienced.</t>
+          <t>A device, tool or apparatus used to obtain, measure and/or analyze data.</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -1306,21 +1340,22 @@
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>datacite:Journal</t>
+          <t>datacite:InteractiveResource</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Journal</t>
+          <t>InteractiveResource</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>A scholarly publication consisting of articles that is published regularly throughout the year.</t>
+          <t>A resource requiring interaction from the user to be understood, executed, or experienced.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -1336,21 +1371,22 @@
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>datacite:JournalArticle</t>
+          <t>datacite:Journal</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>JournalArticle</t>
+          <t>Journal</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>A written composition on a topic of interest, which forms a separate part of a journal.</t>
+          <t>A scholarly publication consisting of articles that is published regularly throughout the year.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -1366,21 +1402,22 @@
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>datacite:Model</t>
+          <t>datacite:JournalArticle</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Model</t>
+          <t>JournalArticle</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>An abstract, conceptual, graphical, mathematical or visualization model that represents empirical objects, phenomena, or physical processes.</t>
+          <t>A written composition on a topic of interest, which forms a separate part of a journal.</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -1396,21 +1433,22 @@
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>datacite:OutputManagementPlan</t>
+          <t>datacite:Model</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>OutputManagementPlan</t>
+          <t>Model</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>A formal document that outlines how research outputs are to be handled both during a research project and after the project is completed.</t>
+          <t>An abstract, conceptual, graphical, mathematical or visualization model that represents empirical objects, phenomena, or physical processes.</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -1426,21 +1464,22 @@
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>datacite:PeerReview</t>
+          <t>datacite:OutputManagementPlan</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>PeerReview</t>
+          <t>OutputManagementPlan</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Evaluation of scientific, academic, or professional work by others working in the same field.</t>
+          <t>A formal document that outlines how research outputs are to be handled both during a research project and after the project is completed.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -1456,21 +1495,22 @@
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>datacite:PhysicalObject</t>
+          <t>datacite:PeerReview</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>PhysicalObject</t>
+          <t>PeerReview</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>A physical object or substance.</t>
+          <t>Evaluation of scientific, academic, or professional work by others working in the same field.</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -1486,21 +1526,22 @@
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>datacite:Preprint</t>
+          <t>datacite:PhysicalObject</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Preprint</t>
+          <t>PhysicalObject</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>A version of a scholarly or scientific paper that precedes formal peer review and publication in a peer-reviewed scholarly or scientific journal.</t>
+          <t>A physical object or substance.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -1516,21 +1557,22 @@
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>datacite:Report</t>
+          <t>datacite:Preprint</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Report</t>
+          <t>Preprint</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>A document that presents information in an organized format for a specific audience and purpose.</t>
+          <t>A version of a scholarly or scientific paper that precedes formal peer review and publication in a peer-reviewed scholarly or scientific journal.</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -1546,21 +1588,22 @@
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>datacite:Service</t>
+          <t>datacite:Report</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Service</t>
+          <t>Report</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>An organized system of apparatus, appliances, staff, etc., for supplying some function(s) required by end users.</t>
+          <t>A document that presents information in an organized format for a specific audience and purpose.</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -1576,21 +1619,22 @@
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>datacite:Software</t>
+          <t>datacite:Service</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Service</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>A computer program other than a computational notebook, in either source code (text) or compiled form. Use this type for general software components supporting scholarly research. Use the “ComputationalNotebook” value for virtual notebooks.</t>
+          <t>An organized system of apparatus, appliances, staff, etc., for supplying some function(s) required by end users.</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -1606,21 +1650,22 @@
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>datacite:Sound</t>
+          <t>datacite:Software</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Sound</t>
+          <t>Software</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>A resource primarily intended to be heard.</t>
+          <t>A computer program other than a computational notebook, in either source code (text) or compiled form. Use this type for general software components supporting scholarly research. Use the “ComputationalNotebook” value for virtual notebooks.</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -1636,21 +1681,22 @@
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>datacite:Standard</t>
+          <t>datacite:Sound</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Standard</t>
+          <t>Sound</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Something established by authority, custom, or general consent as a model, example, or point of reference.</t>
+          <t>A resource primarily intended to be heard.</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
@@ -1666,21 +1712,22 @@
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>datacite:StudyRegistration</t>
+          <t>datacite:Standard</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>StudyRegistration</t>
+          <t>Standard</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>A detailed, time-stamped description of a research plan, often openly shared in a registry or published in a journal before the study is conducted to lend accountability and transparency in the hypothesis generating and testing process.</t>
+          <t>Something established by authority, custom, or general consent as a model, example, or point of reference.</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -1696,21 +1743,22 @@
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>datacite:Text</t>
+          <t>datacite:StudyRegistration</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>StudyRegistration</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>A resource consisting primarily of words for reading that is not covered by any other textual resource type in this list.</t>
+          <t>A detailed, time-stamped description of a research plan, often openly shared in a registry or published in a journal before the study is conducted to lend accountability and transparency in the hypothesis generating and testing process.</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
@@ -1726,21 +1774,22 @@
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>datacite:Workflow</t>
+          <t>datacite:Text</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Workflow</t>
+          <t>Text</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>A structured series of steps which can be executed to produce a final outcome, allowing users a means to specify and enact their work in a more reproducible manner.</t>
+          <t>A resource consisting primarily of words for reading that is not covered by any other textual resource type in this list.</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
@@ -1756,21 +1805,22 @@
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>datacite:Other</t>
+          <t>datacite:Workflow</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Workflow</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>If selected, supply a value for ResourceType.</t>
+          <t>A structured series of steps which can be executed to produce a final outcome, allowing users a means to specify and enact their work in a more reproducible manner.</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
@@ -1786,86 +1836,85 @@
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>datacite:relatedIdentifierType</t>
+          <t>datacite:OtherResourceType</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>relatedIdentifierType</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>The type of the RelatedIdentifier.</t>
+          <t>If selected, supply a value for ResourceType.</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr"/>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>datacite:resourceTypeGeneral</t>
+        </is>
+      </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>datacite:ARK</t>
+          <t>datacite:relatedIdentifierType</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ARK</t>
+          <t>relatedIdentifierType</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>A URI designed to support long-term access to information objects. In general, ARK syntax is of the form (brackets, []. indicate optional elements: [http://NMA/]ark:/NAAN/Name [Qualifier]</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Archival Resource Key</t>
-        </is>
-      </c>
+          <t>The type of the RelatedIdentifier.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>datacite:relatedIdentifierType</t>
-        </is>
-      </c>
+      <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>datacite:arXiv</t>
+          <t>datacite:ARK</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>arXiv</t>
+          <t>ARK</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>arXiv.org is a repository of preprints of scientific papers in the fields of mathematics, physics, astronomy, computer science, quantitative biology, statistics, and quantitative finance.</t>
+          <t>A URI designed to support long-term access to information objects. In general, ARK syntax is of the form (brackets, []. indicate optional elements: [http://NMA/]ark:/NAAN/Name [Qualifier]</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>arXiv identifier</t>
+          <t>Archival Resource Key</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -1880,26 +1929,27 @@
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>datacite:bibcode</t>
+          <t>datacite:arXiv</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>bibcode</t>
+          <t>arXiv</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>A standardized 19-character identifier according to the syntax yyyyjjjjjvvvvmppppa. See http://info-uri.info/registry/OAIHandler?verb=GetRecord&amp;metadataPrefix=reg&amp;identifier=info:bibcode/.</t>
+          <t>arXiv.org is a repository of preprints of scientific papers in the fields of mathematics, physics, astronomy, computer science, quantitative biology, statistics, and quantitative finance.</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Astrophysics Data System bibliographic codes</t>
+          <t>arXiv identifier</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -1914,26 +1964,27 @@
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>datacite:DOI</t>
+          <t>datacite:bibcode</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>DOI</t>
+          <t>bibcode</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>A character string used to uniquely identify an object. A DOI name is divided into two parts, a prefix and a suffix, separated by a slash.</t>
+          <t>A standardized 19-character identifier according to the syntax yyyyjjjjjvvvvmppppa. See http://info-uri.info/registry/OAIHandler?verb=GetRecord&amp;metadataPrefix=reg&amp;identifier=info:bibcode/.</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Digital Object Identifier</t>
+          <t>Astrophysics Data System bibliographic codes</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -1948,26 +1999,27 @@
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>datacite:EAN13</t>
+          <t>datacite:DOI</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>EAN13</t>
+          <t>DOI</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>A 13-digit barcoding standard that is a superset of the original 12-digit Universal Product Code (UPC) system.</t>
+          <t>A character string used to uniquely identify an object. A DOI name is divided into two parts, a prefix and a suffix, separated by a slash.</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>European Article Number (now renamed International Article Number, but retaining the original acronym)</t>
+          <t>Digital Object Identifier</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -1982,26 +2034,27 @@
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>datacite:EISSN</t>
+          <t>datacite:EAN13</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>EISSN</t>
+          <t>EAN13</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>ISSN used to identify periodicals in electronic form (eISSN or e-ISSN).</t>
+          <t>A 13-digit barcoding standard that is a superset of the original 12-digit Universal Product Code (UPC) system.</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>A 13-digit barcoding standard that is a superset of the original 12-digit Universal Product Code (UPC) system.</t>
+          <t>European Article Number (now renamed International Article Number, but retaining the original acronym)</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -2016,26 +2069,27 @@
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>datacite:Handle</t>
+          <t>datacite:EISSN</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Handle</t>
+          <t>EISSN</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>This refers specifically to an ID in the Handle system operated by the Corporation for National Research Initiatives (CNRI).</t>
+          <t>ISSN used to identify periodicals in electronic form (eISSN or e-ISSN).</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Handle</t>
+          <t>A 13-digit barcoding standard that is a superset of the original 12-digit Universal Product Code (UPC) system.</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -2050,26 +2104,27 @@
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>datacite:IGSN</t>
+          <t>datacite:Handle</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>IGSN</t>
+          <t>Handle</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>A code that uniquely identifies samples from our natural environment and related features-of-interest.</t>
+          <t>This refers specifically to an ID in the Handle system operated by the Corporation for National Research Initiatives (CNRI).</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>International Generic Sample Number</t>
+          <t>Handle</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -2084,26 +2139,27 @@
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>datacite:ISBN</t>
+          <t>datacite:IGSN</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>ISBN</t>
+          <t>IGSN</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>A unique numeric book identifier. There are 2 formats: a 10-digit ISBN format and a 13-digit ISBN.</t>
+          <t>A code that uniquely identifies samples from our natural environment and related features-of-interest.</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>International Standard Book Number</t>
+          <t>International Generic Sample Number</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
@@ -2118,26 +2174,27 @@
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>datacite:ISSN</t>
+          <t>datacite:ISBN</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ISSN</t>
+          <t>ISBN</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>A unique 8-digit number used to identify a print or electronic periodical publication.</t>
+          <t>A unique numeric book identifier. There are 2 formats: a 10-digit ISBN format and a 13-digit ISBN.</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>International Standard Serial Number</t>
+          <t>International Standard Book Number</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
@@ -2152,26 +2209,27 @@
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>datacite:ISTC</t>
+          <t>datacite:ISSN</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ISTC</t>
+          <t>ISSN</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>A unique “number” assigned to a textual work. An ISTC consists of 16 numbers and/or letters.</t>
+          <t>A unique 8-digit number used to identify a print or electronic periodical publication.</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>International Standard Text Code</t>
+          <t>International Standard Serial Number</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -2186,26 +2244,27 @@
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>datacite:LISSN</t>
+          <t>datacite:ISTC</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>LISSN</t>
+          <t>ISTC</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>The linking ISSN or ISSN-L enables collocation or linking among different media versions of a continuing resource.</t>
+          <t>A unique “number” assigned to a textual work. An ISTC consists of 16 numbers and/or letters.</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Linking ISSN</t>
+          <t>International Standard Text Code</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
@@ -2220,6 +2279,7 @@
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2234,12 +2294,12 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>A unique identifier for data in the Life Science domain. Format: urn:lsid:authority:namespace:identifier:revision.</t>
+          <t>The linking ISSN or ISSN-L enables collocation or linking among different media versions of a continuing resource.</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Life Science Identifiers</t>
+          <t>Linking ISSN</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
@@ -2254,26 +2314,27 @@
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>datacite:PMID</t>
+          <t>datacite:LISSN</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>PMID</t>
+          <t>LISSN</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>A unique number assigned to each PubMed record.</t>
+          <t>A unique identifier for data in the Life Science domain. Format: urn:lsid:authority:namespace:identifier:revision.</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>PubMed identifier</t>
+          <t>Life Science Identifiers</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
@@ -2288,26 +2349,27 @@
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>datacite:PURL</t>
+          <t>datacite:PMID</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>PURL</t>
+          <t>PMID</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>A PURL has three parts: (1) a protocol, (2) a resolver address, and (3) a name.</t>
+          <t>A unique number assigned to each PubMed record.</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Persistent Uniform Resource Locator</t>
+          <t>PubMed identifier</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
@@ -2322,26 +2384,27 @@
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>datacite:UPC</t>
+          <t>datacite:PURL</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>UPC</t>
+          <t>PURL</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>A barcode symbology used for tracking trade items in stores. Its most common form, the UPC-A, consists of 12 numerical digits.</t>
+          <t>A PURL has three parts: (1) a protocol, (2) a resolver address, and (3) a name.</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Universal Product Code</t>
+          <t>Persistent Uniform Resource Locator</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
@@ -2356,26 +2419,27 @@
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr"/>
       <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>datacite:URL</t>
+          <t>datacite:UPC</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>URL</t>
+          <t>UPC</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Also known as web address, a URL is a specific character string that constitutes a reference to a resource. The syntax is: scheme://domain:port/path?query_string#fragment_id.</t>
+          <t>A barcode symbology used for tracking trade items in stores. Its most common form, the UPC-A, consists of 12 numerical digits.</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Uniform Resource Locator</t>
+          <t>Universal Product Code</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -2390,26 +2454,27 @@
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
       <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>datacite:URN</t>
+          <t>datacite:URL</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>URN</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>A unique and persistent identifier of an electronic document. The syntax is: urn:&lt;NID&gt;:&lt;NSS&gt;. The leading urn: sequence is case-insensitive, &lt;NID&gt; is the namespace identifier, &lt;NSS&gt; is the namespace-specific string.</t>
+          <t>Also known as web address, a URL is a specific character string that constitutes a reference to a resource. The syntax is: scheme://domain:port/path?query_string#fragment_id.</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Uniform Resource Name</t>
+          <t>Uniform Resource Locator</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
@@ -2424,26 +2489,27 @@
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>datacite:w3id</t>
+          <t>datacite:URN</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>w3id</t>
+          <t>URN</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Mostly used to publish vocabularies and ontologies. The letters ‘w3’ stand for “World Wide Web”.</t>
+          <t>A unique and persistent identifier of an electronic document. The syntax is: urn:&lt;NID&gt;:&lt;NSS&gt;. The leading urn: sequence is case-insensitive, &lt;NID&gt; is the namespace identifier, &lt;NSS&gt; is the namespace-specific string.</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Permanent identifier for Web applications</t>
+          <t>Uniform Resource Name</t>
         </is>
       </c>
       <c r="E67" t="inlineStr"/>
@@ -2458,77 +2524,84 @@
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr"/>
       <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>datacite:relationType</t>
+          <t>datacite:w3id</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>relationType</t>
+          <t>w3id</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Description of the relationship of the resource being registered (A) and the related resource (B).</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr"/>
+          <t>Mostly used to publish vocabularies and ontologies. The letters ‘w3’ stand for “World Wide Web”.</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Permanent identifier for Web applications</t>
+        </is>
+      </c>
       <c r="E68" t="inlineStr"/>
-      <c r="F68" t="inlineStr"/>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>datacite:relatedIdentifierType</t>
+        </is>
+      </c>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr"/>
       <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>datacite:IsCitedBy</t>
+          <t>datacite:relationType</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>IsCitedBy</t>
+          <t>relationType</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>indicates that B includes A in a citation</t>
+          <t>Description of the relationship of the resource being registered (A) and the related resource (B).</t>
         </is>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>datacite:relationType</t>
-        </is>
-      </c>
+      <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="inlineStr"/>
       <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>datacite:Cites</t>
+          <t>datacite:IsCitedBy</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Cites</t>
+          <t>IsCitedBy</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>indicates that A includes B in a citation</t>
+          <t>indicates that B includes A in a citation</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
@@ -2544,21 +2617,22 @@
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr"/>
       <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>datacite:IsSupplementTo</t>
+          <t>datacite:Cites</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>IsSupplementTo</t>
+          <t>Cites</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>indicates that A is a supplement to B</t>
+          <t>indicates that A includes B in a citation</t>
         </is>
       </c>
       <c r="D71" t="inlineStr"/>
@@ -2574,21 +2648,22 @@
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>datacite:IsSupplementedBy</t>
+          <t>datacite:IsSupplementTo</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>IsSupplementedBy</t>
+          <t>IsSupplementTo</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>indicates that B is a supplement to A</t>
+          <t>indicates that A is a supplement to B</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
@@ -2604,21 +2679,22 @@
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>datacite:IsContinuedBy</t>
+          <t>datacite:IsSupplementedBy</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>IsContinuedBy</t>
+          <t>IsSupplementedBy</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>indicates A is continued by the work B</t>
+          <t>indicates that B is a supplement to A</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
@@ -2634,21 +2710,22 @@
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>datacite:Continues</t>
+          <t>datacite:IsContinuedBy</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Continues</t>
+          <t>IsContinuedBy</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>indicates A is a continuation of the work B</t>
+          <t>indicates A is continued by the work B</t>
         </is>
       </c>
       <c r="D74" t="inlineStr"/>
@@ -2664,21 +2741,22 @@
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>datacite:Describes</t>
+          <t>datacite:Continues</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Describes</t>
+          <t>Continues</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>indicates A describes B</t>
+          <t>indicates A is a continuation of the work B</t>
         </is>
       </c>
       <c r="D75" t="inlineStr"/>
@@ -2694,21 +2772,22 @@
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr"/>
+      <c r="M75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>datacite:IsDescribedBy</t>
+          <t>datacite:Describes</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>IsDescribedBy</t>
+          <t>Describes</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>indicates A is described by B</t>
+          <t>indicates A describes B</t>
         </is>
       </c>
       <c r="D76" t="inlineStr"/>
@@ -2724,21 +2803,22 @@
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>datacite:HasMetadata</t>
+          <t>datacite:IsDescribedBy</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>HasMetadata</t>
+          <t>IsDescribedBy</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>indicates resource A has additional metadata B</t>
+          <t>indicates A is described by B</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
@@ -2754,21 +2834,22 @@
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr"/>
+      <c r="M77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>datacite:IsMetadataFor</t>
+          <t>datacite:HasMetadata</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>IsMetadataFor</t>
+          <t>HasMetadata</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>indicates additional metadata A for a resource B</t>
+          <t>indicates resource A has additional metadata B</t>
         </is>
       </c>
       <c r="D78" t="inlineStr"/>
@@ -2784,21 +2865,22 @@
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr"/>
+      <c r="M78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>datacite:HasVersion</t>
+          <t>datacite:IsMetadataFor</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>HasVersion</t>
+          <t>IsMetadataFor</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>indicates A has a version B</t>
+          <t>indicates additional metadata A for a resource B</t>
         </is>
       </c>
       <c r="D79" t="inlineStr"/>
@@ -2814,22 +2896,22 @@
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr"/>
+      <c r="M79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>datacite:IsVersionOf</t>
+          <t>datacite:HasVersion</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>IsVersionOf</t>
+          <t>HasVersion</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t xml:space="preserve">indicates A is a version of B
-</t>
+          <t>indicates A has a version B</t>
         </is>
       </c>
       <c r="D80" t="inlineStr"/>
@@ -2845,21 +2927,23 @@
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr"/>
+      <c r="M80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>datacite:IsNewVersionOf</t>
+          <t>datacite:IsVersionOf</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>IsNewVersionOf</t>
+          <t>IsVersionOf</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>indicates A is a new edition of B, where the new edition has been modified or updated</t>
+          <t xml:space="preserve">indicates A is a version of B
+</t>
         </is>
       </c>
       <c r="D81" t="inlineStr"/>
@@ -2875,21 +2959,22 @@
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>datacite:IsPreviousVersionOf</t>
+          <t>datacite:IsNewVersionOf</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>IsPreviousVersion Of</t>
+          <t>IsNewVersionOf</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>indicates A is a previous edition of B</t>
+          <t>indicates A is a new edition of B, where the new edition has been modified or updated</t>
         </is>
       </c>
       <c r="D82" t="inlineStr"/>
@@ -2905,21 +2990,22 @@
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr"/>
       <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>datacite:IsPartOf</t>
+          <t>datacite:IsPreviousVersionOf</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>IsPartOf</t>
+          <t>IsPreviousVersion Of</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>indicates A is a portion of B; may be used for elements of a series</t>
+          <t>indicates A is a previous edition of B</t>
         </is>
       </c>
       <c r="D83" t="inlineStr"/>
@@ -2935,21 +3021,22 @@
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="inlineStr"/>
       <c r="L83" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>datacite:HasPart</t>
+          <t>datacite:IsPartOf</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>HasPart</t>
+          <t>IsPartOf</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>indicates A includes the part B</t>
+          <t>indicates A is a portion of B; may be used for elements of a series</t>
         </is>
       </c>
       <c r="D84" t="inlineStr"/>
@@ -2965,21 +3052,22 @@
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>datacite:IsPublishedIn</t>
+          <t>datacite:HasPart</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>IsPublishedIn</t>
+          <t>HasPart</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>indicates A is published inside B, but is independent of other things published inside of B</t>
+          <t>indicates A includes the part B</t>
         </is>
       </c>
       <c r="D85" t="inlineStr"/>
@@ -2995,21 +3083,22 @@
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr"/>
+      <c r="M85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>datacite:IsReferencedBy</t>
+          <t>datacite:IsPublishedIn</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>IsReferencedBy</t>
+          <t>IsPublishedIn</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>indicates A is used as a source of information by B</t>
+          <t>indicates A is published inside B, but is independent of other things published inside of B</t>
         </is>
       </c>
       <c r="D86" t="inlineStr"/>
@@ -3025,21 +3114,22 @@
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr"/>
+      <c r="M86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>datacite:References</t>
+          <t>datacite:IsReferencedBy</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>References</t>
+          <t>IsReferencedBy</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>indicates B is used as a source of information for A</t>
+          <t>indicates A is used as a source of information by B</t>
         </is>
       </c>
       <c r="D87" t="inlineStr"/>
@@ -3055,21 +3145,22 @@
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr"/>
+      <c r="M87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>datacite:IsDocumentedBy</t>
+          <t>datacite:References</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>IsDocumentedBy</t>
+          <t>References</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>indicates B is documentation about/explaining A</t>
+          <t>indicates B is used as a source of information for A</t>
         </is>
       </c>
       <c r="D88" t="inlineStr"/>
@@ -3085,21 +3176,22 @@
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr"/>
       <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>datacite:Documents</t>
+          <t>datacite:IsDocumentedBy</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Documents</t>
+          <t>IsDocumentedBy</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>indicates A is documentation about/explaining B</t>
+          <t>indicates B is documentation about/explaining A</t>
         </is>
       </c>
       <c r="D89" t="inlineStr"/>
@@ -3115,21 +3207,22 @@
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>datacite:IsCompiledBy</t>
+          <t>datacite:Documents</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>IsCompiledBy</t>
+          <t>Documents</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>indicates B is used to compile or create A</t>
+          <t>indicates A is documentation about/explaining B</t>
         </is>
       </c>
       <c r="D90" t="inlineStr"/>
@@ -3145,22 +3238,22 @@
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>datacite:Compiles</t>
+          <t>datacite:IsCompiledBy</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Compiles</t>
+          <t>IsCompiledBy</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t xml:space="preserve">indicates B is the result of a compile or creation event using A
-</t>
+          <t>indicates B is used to compile or create A</t>
         </is>
       </c>
       <c r="D91" t="inlineStr"/>
@@ -3176,21 +3269,23 @@
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="inlineStr"/>
       <c r="L91" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>datacite:IsVariantFormOf</t>
+          <t>datacite:Compiles</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>IsVariantFormOf</t>
+          <t>Compiles</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>indicates A is a variant or different form of B</t>
+          <t xml:space="preserve">indicates B is the result of a compile or creation event using A
+</t>
         </is>
       </c>
       <c r="D92" t="inlineStr"/>
@@ -3206,21 +3301,22 @@
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr"/>
       <c r="L92" t="inlineStr"/>
+      <c r="M92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>datacite:IsOriginalFormOf</t>
+          <t>datacite:IsVariantFormOf</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>IsOriginalFormOf</t>
+          <t>IsVariantFormOf</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>indicates A is the original form of B</t>
+          <t>indicates A is a variant or different form of B</t>
         </is>
       </c>
       <c r="D93" t="inlineStr"/>
@@ -3236,22 +3332,22 @@
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr"/>
       <c r="L93" t="inlineStr"/>
+      <c r="M93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>datacite:IsIdenticalTo</t>
+          <t>datacite:IsOriginalFormOf</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>IsIdenticalTo</t>
+          <t>IsOriginalFormOf</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t xml:space="preserve">indicates that A is identical to B, for use when there is a need to register two separate instances of the same resource
-</t>
+          <t>indicates A is the original form of B</t>
         </is>
       </c>
       <c r="D94" t="inlineStr"/>
@@ -3267,21 +3363,23 @@
       <c r="J94" t="inlineStr"/>
       <c r="K94" t="inlineStr"/>
       <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>datacite:IsReviewedBy</t>
+          <t>datacite:IsIdenticalTo</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>IsReviewedBy</t>
+          <t>IsIdenticalTo</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>indicates that A is reviewed by B</t>
+          <t xml:space="preserve">indicates that A is identical to B, for use when there is a need to register two separate instances of the same resource
+</t>
         </is>
       </c>
       <c r="D95" t="inlineStr"/>
@@ -3297,21 +3395,22 @@
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr"/>
       <c r="L95" t="inlineStr"/>
+      <c r="M95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>datacite:Reviews</t>
+          <t>datacite:IsReviewedBy</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Reviews</t>
+          <t>IsReviewedBy</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>indicates that A is a review of B</t>
+          <t>indicates that A is reviewed by B</t>
         </is>
       </c>
       <c r="D96" t="inlineStr"/>
@@ -3327,21 +3426,22 @@
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="inlineStr"/>
       <c r="L96" t="inlineStr"/>
+      <c r="M96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>datacite:IsDerivedFrom</t>
+          <t>datacite:Reviews</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>IsDerivedFrom</t>
+          <t>Reviews</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>indicates B is a source upon which A is based</t>
+          <t>indicates that A is a review of B</t>
         </is>
       </c>
       <c r="D97" t="inlineStr"/>
@@ -3357,21 +3457,22 @@
       <c r="J97" t="inlineStr"/>
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="inlineStr"/>
+      <c r="M97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>datacite:IsSourceOf</t>
+          <t>datacite:IsDerivedFrom</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>IsSourceOf</t>
+          <t>IsDerivedFrom</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>indicates A is a source upon which B is based</t>
+          <t>indicates B is a source upon which A is based</t>
         </is>
       </c>
       <c r="D98" t="inlineStr"/>
@@ -3387,21 +3488,22 @@
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>datacite:IsRequiredBy</t>
+          <t>datacite:IsSourceOf</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>IsRequiredBy</t>
+          <t>IsSourceOf</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Indicates A is required by B</t>
+          <t>indicates A is a source upon which B is based</t>
         </is>
       </c>
       <c r="D99" t="inlineStr"/>
@@ -3417,21 +3519,22 @@
       <c r="J99" t="inlineStr"/>
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>datacite:Requires</t>
+          <t>datacite:IsRequiredBy</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Requires</t>
+          <t>IsRequiredBy</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Indicates A requires B</t>
+          <t>Indicates A is required by B</t>
         </is>
       </c>
       <c r="D100" t="inlineStr"/>
@@ -3447,21 +3550,22 @@
       <c r="J100" t="inlineStr"/>
       <c r="K100" t="inlineStr"/>
       <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>datacite:Obsoletes</t>
+          <t>datacite:Requires</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Obsoletes</t>
+          <t>Requires</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Indicates A replaces B</t>
+          <t>Indicates A requires B</t>
         </is>
       </c>
       <c r="D101" t="inlineStr"/>
@@ -3477,21 +3581,22 @@
       <c r="J101" t="inlineStr"/>
       <c r="K101" t="inlineStr"/>
       <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>datacite:IsRequiredBy</t>
+          <t>datacite:Obsoletes</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>IsRequiredBy</t>
+          <t>Obsoletes</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Indicates A is replaced by B</t>
+          <t>Indicates A replaces B</t>
         </is>
       </c>
       <c r="D102" t="inlineStr"/>
@@ -3507,21 +3612,22 @@
       <c r="J102" t="inlineStr"/>
       <c r="K102" t="inlineStr"/>
       <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>datacite:IsCollectedBy</t>
+          <t>datacite:IsRequiredBy</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>IsCollectedBy</t>
+          <t>IsRequiredBy</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Indicates A is collected by B</t>
+          <t>Indicates A is replaced by B</t>
         </is>
       </c>
       <c r="D103" t="inlineStr"/>
@@ -3537,21 +3643,22 @@
       <c r="J103" t="inlineStr"/>
       <c r="K103" t="inlineStr"/>
       <c r="L103" t="inlineStr"/>
+      <c r="M103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>datacite:Collects</t>
+          <t>datacite:IsCollectedBy</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Collects</t>
+          <t>IsCollectedBy</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Indicates A collects B</t>
+          <t>Indicates A is collected by B</t>
         </is>
       </c>
       <c r="D104" t="inlineStr"/>
@@ -3567,77 +3674,80 @@
       <c r="J104" t="inlineStr"/>
       <c r="K104" t="inlineStr"/>
       <c r="L104" t="inlineStr"/>
+      <c r="M104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>datacite:descriptionType</t>
+          <t>datacite:Collects</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>descriptionType</t>
+          <t>Collects</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>The type of the Description.</t>
+          <t>Indicates A collects B</t>
         </is>
       </c>
       <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr"/>
-      <c r="F105" t="inlineStr"/>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>datacite:relationType</t>
+        </is>
+      </c>
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr"/>
       <c r="K105" t="inlineStr"/>
       <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>datacite:Abstract</t>
+          <t>datacite:descriptionType</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Abstract</t>
+          <t>descriptionType</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>A brief description of the resource and the context in which the resource was created.</t>
+          <t>The type of the Description.</t>
         </is>
       </c>
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr"/>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>datacite:descriptionType</t>
-        </is>
-      </c>
+      <c r="F106" t="inlineStr"/>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="inlineStr"/>
       <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr"/>
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>datacite:Methods</t>
+          <t>datacite:Abstract</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Methods</t>
+          <t>Abstract</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>The methodology employed for the study or research.</t>
+          <t>A brief description of the resource and the context in which the resource was created.</t>
         </is>
       </c>
       <c r="D107" t="inlineStr"/>
@@ -3653,21 +3763,22 @@
       <c r="J107" t="inlineStr"/>
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>datacite:SeriesInformation</t>
+          <t>datacite:Methods</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>SeriesInformation</t>
+          <t>Methods</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Information about a repeating series, such as volume, issue, number.</t>
+          <t>The methodology employed for the study or research.</t>
         </is>
       </c>
       <c r="D108" t="inlineStr"/>
@@ -3683,21 +3794,22 @@
       <c r="J108" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>datacite:TableOfContents</t>
+          <t>datacite:SeriesInformation</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>TableOfContents</t>
+          <t>SeriesInformation</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>A listing of the Table of Contents.</t>
+          <t>Information about a repeating series, such as volume, issue, number.</t>
         </is>
       </c>
       <c r="D109" t="inlineStr"/>
@@ -3713,21 +3825,22 @@
       <c r="J109" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>datacite:TechnicalInfo</t>
+          <t>datacite:TableOfContents</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>TechnicalInfo</t>
+          <t>TableOfContents</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Detailed information that may be associated with design, implementation, operation, use, and/or maintenance of a process, system, or instrument.</t>
+          <t>A listing of the Table of Contents.</t>
         </is>
       </c>
       <c r="D110" t="inlineStr"/>
@@ -3743,21 +3856,22 @@
       <c r="J110" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
       <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>datacite:OtherDescriptionType</t>
+          <t>datacite:TechnicalInfo</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>TechnicalInfo</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Other description information that does not fit into an existing category.</t>
+          <t>Detailed information that may be associated with design, implementation, operation, use, and/or maintenance of a process, system, or instrument.</t>
         </is>
       </c>
       <c r="D111" t="inlineStr"/>
@@ -3773,72 +3887,75 @@
       <c r="J111" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
       <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>datacite:dateType</t>
+          <t>datacite:OtherDescriptionType</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>dateType</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>The type of date. Use RKMS‐ISO8601 standard for depicting date ranges.To indicate the end of an embargo period, use Available. To indicate the start of an embargo period, use Submitted or Accepted, as appropriate.</t>
+          <t>Other description information that does not fit into an existing category.</t>
         </is>
       </c>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
-      <c r="F112" t="inlineStr"/>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>datacite:descriptionType</t>
+        </is>
+      </c>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="inlineStr"/>
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>datacite:Accepted</t>
+          <t>datacite:dateType</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Accepted</t>
+          <t>dateType</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>The date that the publisher accepted the resource into their system.</t>
+          <t>The type of date. Use RKMS‐ISO8601 standard for depicting date ranges.To indicate the end of an embargo period, use Available. To indicate the start of an embargo period, use Submitted or Accepted, as appropriate.</t>
         </is>
       </c>
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>datacite:dateType</t>
-        </is>
-      </c>
+      <c r="F113" t="inlineStr"/>
       <c r="G113" t="inlineStr"/>
       <c r="H113" t="inlineStr"/>
       <c r="I113" t="inlineStr"/>
       <c r="J113" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>datacite:Available</t>
+          <t>datacite:Accepted</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>Accepted</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3859,21 +3976,22 @@
       <c r="J114" t="inlineStr"/>
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>datacite:Copyrighted</t>
+          <t>datacite:Available</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Copyrighted</t>
+          <t>Available</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>The specific, documented date at which the resource receives a copyrighted status, if applicable.</t>
+          <t>The date that the publisher accepted the resource into their system.</t>
         </is>
       </c>
       <c r="D115" t="inlineStr"/>
@@ -3889,21 +4007,22 @@
       <c r="J115" t="inlineStr"/>
       <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>datacite:Collected</t>
+          <t>datacite:Copyrighted</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Collected</t>
+          <t>Copyrighted</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>The date or date range in which the resource content was collected.</t>
+          <t>The specific, documented date at which the resource receives a copyrighted status, if applicable.</t>
         </is>
       </c>
       <c r="D116" t="inlineStr"/>
@@ -3919,21 +4038,22 @@
       <c r="J116" t="inlineStr"/>
       <c r="K116" t="inlineStr"/>
       <c r="L116" t="inlineStr"/>
+      <c r="M116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>datacite:Created</t>
+          <t>datacite:Collected</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Created</t>
+          <t>Collected</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>The date the resource itself was put together; this could refer to a timeframe in ancient history, a date range, or a single date for a final component, e.g., the finalised file with all the data.</t>
+          <t>The date or date range in which the resource content was collected.</t>
         </is>
       </c>
       <c r="D117" t="inlineStr"/>
@@ -3949,21 +4069,22 @@
       <c r="J117" t="inlineStr"/>
       <c r="K117" t="inlineStr"/>
       <c r="L117" t="inlineStr"/>
+      <c r="M117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>datacite:Issued</t>
+          <t>datacite:Created</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Issued</t>
+          <t>Created</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>The date that the resource is published or distributed, e.g., to a data centre.</t>
+          <t>The date the resource itself was put together; this could refer to a timeframe in ancient history, a date range, or a single date for a final component, e.g., the finalised file with all the data.</t>
         </is>
       </c>
       <c r="D118" t="inlineStr"/>
@@ -3979,21 +4100,22 @@
       <c r="J118" t="inlineStr"/>
       <c r="K118" t="inlineStr"/>
       <c r="L118" t="inlineStr"/>
+      <c r="M118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>datacite:OtherDateType</t>
+          <t>datacite:Issued</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Issued</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Other date that does not fit into an existing category.</t>
+          <t>The date that the resource is published or distributed, e.g., to a data centre.</t>
         </is>
       </c>
       <c r="D119" t="inlineStr"/>
@@ -4009,21 +4131,22 @@
       <c r="J119" t="inlineStr"/>
       <c r="K119" t="inlineStr"/>
       <c r="L119" t="inlineStr"/>
+      <c r="M119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>datacite:Submitted</t>
+          <t>datacite:OtherDateType</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>The date the creator submits the resource to the publisher. This could be different from Accepted if the publisher then applies a selection process.</t>
+          <t>Other date that does not fit into an existing category.</t>
         </is>
       </c>
       <c r="D120" t="inlineStr"/>
@@ -4039,21 +4162,22 @@
       <c r="J120" t="inlineStr"/>
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr"/>
+      <c r="M120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>datacite:Updated</t>
+          <t>datacite:Submitted</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Updated</t>
+          <t>Submitted</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>The date of the last update to the resource, when the resource is being added to. May be a range.</t>
+          <t>The date the creator submits the resource to the publisher. This could be different from Accepted if the publisher then applies a selection process.</t>
         </is>
       </c>
       <c r="D121" t="inlineStr"/>
@@ -4069,21 +4193,22 @@
       <c r="J121" t="inlineStr"/>
       <c r="K121" t="inlineStr"/>
       <c r="L121" t="inlineStr"/>
+      <c r="M121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>datacite:Valid</t>
+          <t>datacite:Updated</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Valid</t>
+          <t>Updated</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>The date or date range during which the dataset or resource is accurate.</t>
+          <t>The date of the last update to the resource, when the resource is being added to. May be a range.</t>
         </is>
       </c>
       <c r="D122" t="inlineStr"/>
@@ -4099,21 +4224,22 @@
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr"/>
+      <c r="M122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>datacite:Withdrawn</t>
+          <t>datacite:Valid</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Withdrawn</t>
+          <t>Valid</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>The date the resource is removed.</t>
+          <t>The date or date range during which the dataset or resource is accurate.</t>
         </is>
       </c>
       <c r="D123" t="inlineStr"/>
@@ -4129,77 +4255,80 @@
       <c r="J123" t="inlineStr"/>
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr"/>
+      <c r="M123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>datacite:contributorType</t>
+          <t>datacite:Withdrawn</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>contributorType</t>
+          <t>Withdrawn</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>The type of contributor of the resource.</t>
+          <t>The date the resource is removed.</t>
         </is>
       </c>
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr"/>
-      <c r="F124" t="inlineStr"/>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>datacite:dateType</t>
+        </is>
+      </c>
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="inlineStr"/>
       <c r="I124" t="inlineStr"/>
       <c r="J124" t="inlineStr"/>
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr"/>
+      <c r="M124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>datacite:ContactPerson</t>
+          <t>datacite:contributorType</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>ContactPerson</t>
+          <t>contributorType</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Person with knowledge of how to access, troubleshoot, or otherwise field issues related to the resource.</t>
+          <t>The type of contributor of the resource.</t>
         </is>
       </c>
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="inlineStr"/>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>datacite:contributorType</t>
-        </is>
-      </c>
+      <c r="F125" t="inlineStr"/>
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="inlineStr"/>
       <c r="I125" t="inlineStr"/>
       <c r="J125" t="inlineStr"/>
       <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr"/>
+      <c r="M125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>datacite:DataCollector</t>
+          <t>datacite:ContactPerson</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>DataCollector</t>
+          <t>ContactPerson</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Person/institution responsible for finding or gathering/collecting data under the guidelines of the author(s) or Principal Investigator (PI).</t>
+          <t>Person with knowledge of how to access, troubleshoot, or otherwise field issues related to the resource.</t>
         </is>
       </c>
       <c r="D126" t="inlineStr"/>
@@ -4215,21 +4344,22 @@
       <c r="J126" t="inlineStr"/>
       <c r="K126" t="inlineStr"/>
       <c r="L126" t="inlineStr"/>
+      <c r="M126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>datacite:DataCurator</t>
+          <t>datacite:DataCollector</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>DataCurator</t>
+          <t>DataCollector</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Person tasked with reviewing, enhancing, cleaning, or standardizing metadata and the associated data submitted for storage, use, and maintenance within a data centre or repository.</t>
+          <t>Person/institution responsible for finding or gathering/collecting data under the guidelines of the author(s) or Principal Investigator (PI).</t>
         </is>
       </c>
       <c r="D127" t="inlineStr"/>
@@ -4245,21 +4375,22 @@
       <c r="J127" t="inlineStr"/>
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr"/>
+      <c r="M127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>datacite:DataManager</t>
+          <t>datacite:DataCurator</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>DataManager</t>
+          <t>DataCurator</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Person (or organisation with a staff of data managers, such as a data centre) responsible for maintaining the finished resource.</t>
+          <t>Person tasked with reviewing, enhancing, cleaning, or standardizing metadata and the associated data submitted for storage, use, and maintenance within a data centre or repository.</t>
         </is>
       </c>
       <c r="D128" t="inlineStr"/>
@@ -4275,21 +4406,22 @@
       <c r="J128" t="inlineStr"/>
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr"/>
+      <c r="M128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>datacite:Distributor</t>
+          <t>datacite:DataManager</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Distributor</t>
+          <t>DataManager</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Institution tasked with responsibility to generate/disseminate copies of the resource in either electronic or print form.</t>
+          <t>Person (or organisation with a staff of data managers, such as a data centre) responsible for maintaining the finished resource.</t>
         </is>
       </c>
       <c r="D129" t="inlineStr"/>
@@ -4305,21 +4437,22 @@
       <c r="J129" t="inlineStr"/>
       <c r="K129" t="inlineStr"/>
       <c r="L129" t="inlineStr"/>
+      <c r="M129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>datacite:Editor</t>
+          <t>datacite:Distributor</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Editor</t>
+          <t>Distributor</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>A person who oversees the details related to the publication format of the resource.</t>
+          <t>Institution tasked with responsibility to generate/disseminate copies of the resource in either electronic or print form.</t>
         </is>
       </c>
       <c r="D130" t="inlineStr"/>
@@ -4335,21 +4468,22 @@
       <c r="J130" t="inlineStr"/>
       <c r="K130" t="inlineStr"/>
       <c r="L130" t="inlineStr"/>
+      <c r="M130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>datacite:HostingInstitution</t>
+          <t>datacite:Editor</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>HostingInstitution</t>
+          <t>Editor</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Typically, the organisation allowing the resource to be available on the internet through the provision of its hardware/software/operating support.</t>
+          <t>A person who oversees the details related to the publication format of the resource.</t>
         </is>
       </c>
       <c r="D131" t="inlineStr"/>
@@ -4365,21 +4499,22 @@
       <c r="J131" t="inlineStr"/>
       <c r="K131" t="inlineStr"/>
       <c r="L131" t="inlineStr"/>
+      <c r="M131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>datacite:Producer</t>
+          <t>datacite:HostingInstitution</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Producer</t>
+          <t>HostingInstitution</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Typically, a person or organisation responsible for the artistry and form of a media product.</t>
+          <t>Typically, the organisation allowing the resource to be available on the internet through the provision of its hardware/software/operating support.</t>
         </is>
       </c>
       <c r="D132" t="inlineStr"/>
@@ -4395,21 +4530,22 @@
       <c r="J132" t="inlineStr"/>
       <c r="K132" t="inlineStr"/>
       <c r="L132" t="inlineStr"/>
+      <c r="M132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>datacite:ProjectLeader</t>
+          <t>datacite:Producer</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>ProjectLeader</t>
+          <t>Producer</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Person officially designated as head of project team or sub- project team instrumental in the work necessary to development of the resource.</t>
+          <t>Typically, a person or organisation responsible for the artistry and form of a media product.</t>
         </is>
       </c>
       <c r="D133" t="inlineStr"/>
@@ -4425,21 +4561,22 @@
       <c r="J133" t="inlineStr"/>
       <c r="K133" t="inlineStr"/>
       <c r="L133" t="inlineStr"/>
+      <c r="M133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>datacite:ProjectManager</t>
+          <t>datacite:ProjectLeader</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>ProjectManager</t>
+          <t>ProjectLeader</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Person officially designated as manager of a project. Project may consist of one or many project teams and sub-teams.</t>
+          <t>Person officially designated as head of project team or sub- project team instrumental in the work necessary to development of the resource.</t>
         </is>
       </c>
       <c r="D134" t="inlineStr"/>
@@ -4455,21 +4592,22 @@
       <c r="J134" t="inlineStr"/>
       <c r="K134" t="inlineStr"/>
       <c r="L134" t="inlineStr"/>
+      <c r="M134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>datacite:ProjectMember</t>
+          <t>datacite:ProjectManager</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>ProjectMember</t>
+          <t>ProjectManager</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Person on the membership list of a designated project/project team.</t>
+          <t>Person officially designated as manager of a project. Project may consist of one or many project teams and sub-teams.</t>
         </is>
       </c>
       <c r="D135" t="inlineStr"/>
@@ -4485,21 +4623,22 @@
       <c r="J135" t="inlineStr"/>
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr"/>
+      <c r="M135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>datacite:RegistrationAgency</t>
+          <t>datacite:ProjectMember</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>RegistrationAgency</t>
+          <t>ProjectMember</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Institution/organisation officially appointed by a Registration Authority to handle specific tasks within a defined area of responsibility.</t>
+          <t>Person on the membership list of a designated project/project team.</t>
         </is>
       </c>
       <c r="D136" t="inlineStr"/>
@@ -4515,21 +4654,22 @@
       <c r="J136" t="inlineStr"/>
       <c r="K136" t="inlineStr"/>
       <c r="L136" t="inlineStr"/>
+      <c r="M136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>datacite:RegistrationAuthority</t>
+          <t>datacite:RegistrationAgency</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>RegistrationAuthority</t>
+          <t>RegistrationAgency</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>A standards-setting body from which Registration Agencies obtain official recognition and guidance.</t>
+          <t>Institution/organisation officially appointed by a Registration Authority to handle specific tasks within a defined area of responsibility.</t>
         </is>
       </c>
       <c r="D137" t="inlineStr"/>
@@ -4545,21 +4685,22 @@
       <c r="J137" t="inlineStr"/>
       <c r="K137" t="inlineStr"/>
       <c r="L137" t="inlineStr"/>
+      <c r="M137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>datacite:RelatedPerson</t>
+          <t>datacite:RegistrationAuthority</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>RelatedPerson</t>
+          <t>RegistrationAuthority</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>A person without a specifically defined role in the development of the resource, but who is someone the author wishes to recognize.</t>
+          <t>A standards-setting body from which Registration Agencies obtain official recognition and guidance.</t>
         </is>
       </c>
       <c r="D138" t="inlineStr"/>
@@ -4575,21 +4716,22 @@
       <c r="J138" t="inlineStr"/>
       <c r="K138" t="inlineStr"/>
       <c r="L138" t="inlineStr"/>
+      <c r="M138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>datacite:Researcher</t>
+          <t>datacite:RelatedPerson</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Researcher</t>
+          <t>RelatedPerson</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>A person involved in analysing data or the results of an experiment or formal study. May indicate an intern or assistant to one of the authors who helped with research but who was not so “key” as to be listed as an author.</t>
+          <t>A person without a specifically defined role in the development of the resource, but who is someone the author wishes to recognize.</t>
         </is>
       </c>
       <c r="D139" t="inlineStr"/>
@@ -4605,21 +4747,22 @@
       <c r="J139" t="inlineStr"/>
       <c r="K139" t="inlineStr"/>
       <c r="L139" t="inlineStr"/>
+      <c r="M139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>datacite:ResearchGroup</t>
+          <t>datacite:Researcher</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>ResearchGroup</t>
+          <t>Researcher</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Typically refers to a group of individuals with a lab, department, or division that has a specifically defined focus of activity.</t>
+          <t>A person involved in analysing data or the results of an experiment or formal study. May indicate an intern or assistant to one of the authors who helped with research but who was not so “key” as to be listed as an author.</t>
         </is>
       </c>
       <c r="D140" t="inlineStr"/>
@@ -4635,21 +4778,22 @@
       <c r="J140" t="inlineStr"/>
       <c r="K140" t="inlineStr"/>
       <c r="L140" t="inlineStr"/>
+      <c r="M140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>datacite:RightsHolder</t>
+          <t>datacite:ResearchGroup</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>RightsHolder</t>
+          <t>ResearchGroup</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Person or institution owning or managing property rights, including intellectual property rights over the resource.</t>
+          <t>Typically refers to a group of individuals with a lab, department, or division that has a specifically defined focus of activity.</t>
         </is>
       </c>
       <c r="D141" t="inlineStr"/>
@@ -4665,21 +4809,22 @@
       <c r="J141" t="inlineStr"/>
       <c r="K141" t="inlineStr"/>
       <c r="L141" t="inlineStr"/>
+      <c r="M141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>datacite:Sponsor</t>
+          <t>datacite:RightsHolder</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Sponsor</t>
+          <t>RightsHolder</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Person or organisation that issued a contract or under the auspices of which a work has been written, printed, published, developed, etc.</t>
+          <t>Person or institution owning or managing property rights, including intellectual property rights over the resource.</t>
         </is>
       </c>
       <c r="D142" t="inlineStr"/>
@@ -4695,21 +4840,22 @@
       <c r="J142" t="inlineStr"/>
       <c r="K142" t="inlineStr"/>
       <c r="L142" t="inlineStr"/>
+      <c r="M142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>datacite:Supervisor</t>
+          <t>datacite:Sponsor</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Supervisor</t>
+          <t>Sponsor</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Designated administrator over one or more groups/teams working to produce a resource, or over one or more steps of a development process.</t>
+          <t>Person or organisation that issued a contract or under the auspices of which a work has been written, printed, published, developed, etc.</t>
         </is>
       </c>
       <c r="D143" t="inlineStr"/>
@@ -4725,21 +4871,22 @@
       <c r="J143" t="inlineStr"/>
       <c r="K143" t="inlineStr"/>
       <c r="L143" t="inlineStr"/>
+      <c r="M143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>datacite:WorkPackageLeader</t>
+          <t>datacite:Supervisor</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>WorkPackageLeader</t>
+          <t>Supervisor</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>A Work Package is a recognized data product, not all of which is included in publication. The package, instead, may include notes, discarded documents, etc. The Work Package Leader is responsible for ensuring the comprehensive contents, versioning, and availability of the Work Package during the development of the resource.</t>
+          <t>Designated administrator over one or more groups/teams working to produce a resource, or over one or more steps of a development process.</t>
         </is>
       </c>
       <c r="D144" t="inlineStr"/>
@@ -4755,21 +4902,22 @@
       <c r="J144" t="inlineStr"/>
       <c r="K144" t="inlineStr"/>
       <c r="L144" t="inlineStr"/>
+      <c r="M144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>datacite:OtherContributorType</t>
+          <t>datacite:WorkPackageLeader</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>WorkPackageLeader</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Any person or institution making a significant contribution to the development and/or maintenance of the resource, but whose contribution is not adequately described by any of the other values for contributorType.</t>
+          <t>A Work Package is a recognized data product, not all of which is included in publication. The package, instead, may include notes, discarded documents, etc. The Work Package Leader is responsible for ensuring the comprehensive contents, versioning, and availability of the Work Package during the development of the resource.</t>
         </is>
       </c>
       <c r="D145" t="inlineStr"/>
@@ -4785,68 +4933,75 @@
       <c r="J145" t="inlineStr"/>
       <c r="K145" t="inlineStr"/>
       <c r="L145" t="inlineStr"/>
+      <c r="M145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>datacite:nameType</t>
+          <t>datacite:OtherContributorType</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>nameType</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>The type of name.</t>
+          <t>Any person or institution making a significant contribution to the development and/or maintenance of the resource, but whose contribution is not adequately described by any of the other values for contributorType.</t>
         </is>
       </c>
       <c r="D146" t="inlineStr"/>
       <c r="E146" t="inlineStr"/>
-      <c r="F146" t="inlineStr"/>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>datacite:contributorType</t>
+        </is>
+      </c>
       <c r="G146" t="inlineStr"/>
       <c r="H146" t="inlineStr"/>
       <c r="I146" t="inlineStr"/>
       <c r="J146" t="inlineStr"/>
       <c r="K146" t="inlineStr"/>
       <c r="L146" t="inlineStr"/>
+      <c r="M146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>datacite:Personal</t>
+          <t>datacite:nameType</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Personal</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr"/>
+          <t>nameType</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>The type of name.</t>
+        </is>
+      </c>
       <c r="D147" t="inlineStr"/>
       <c r="E147" t="inlineStr"/>
-      <c r="F147" t="inlineStr">
-        <is>
-          <t>datacite:nameType</t>
-        </is>
-      </c>
+      <c r="F147" t="inlineStr"/>
       <c r="G147" t="inlineStr"/>
       <c r="H147" t="inlineStr"/>
       <c r="I147" t="inlineStr"/>
       <c r="J147" t="inlineStr"/>
       <c r="K147" t="inlineStr"/>
       <c r="L147" t="inlineStr"/>
+      <c r="M147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>datacite:Organizational</t>
+          <t>datacite:Personal</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Organizational</t>
+          <t>Personal</t>
         </is>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -4863,68 +5018,71 @@
       <c r="J148" t="inlineStr"/>
       <c r="K148" t="inlineStr"/>
       <c r="L148" t="inlineStr"/>
+      <c r="M148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>datacite:titleType</t>
+          <t>datacite:Organizational</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>titleType</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>The type of Title (other than the Main Title).</t>
-        </is>
-      </c>
+          <t>Organizational</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr"/>
       <c r="D149" t="inlineStr"/>
       <c r="E149" t="inlineStr"/>
-      <c r="F149" t="inlineStr"/>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>datacite:nameType</t>
+        </is>
+      </c>
       <c r="G149" t="inlineStr"/>
       <c r="H149" t="inlineStr"/>
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr"/>
       <c r="K149" t="inlineStr"/>
       <c r="L149" t="inlineStr"/>
+      <c r="M149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>datacite:AlternativeTitle</t>
+          <t>datacite:titleType</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>AlternativeTitle</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr"/>
+          <t>titleType</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>The type of Title (other than the Main Title).</t>
+        </is>
+      </c>
       <c r="D150" t="inlineStr"/>
       <c r="E150" t="inlineStr"/>
-      <c r="F150" t="inlineStr">
-        <is>
-          <t>datacite:titleType</t>
-        </is>
-      </c>
+      <c r="F150" t="inlineStr"/>
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="inlineStr"/>
       <c r="I150" t="inlineStr"/>
       <c r="J150" t="inlineStr"/>
       <c r="K150" t="inlineStr"/>
       <c r="L150" t="inlineStr"/>
+      <c r="M150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>datacite:Subtitle</t>
+          <t>datacite:AlternativeTitle</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Subtitle</t>
+          <t>AlternativeTitle</t>
         </is>
       </c>
       <c r="C151" t="inlineStr"/>
@@ -4941,16 +5099,17 @@
       <c r="J151" t="inlineStr"/>
       <c r="K151" t="inlineStr"/>
       <c r="L151" t="inlineStr"/>
+      <c r="M151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>datacite:TranslatedTitle</t>
+          <t>datacite:Subtitle</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>TranslatedTitle</t>
+          <t>Subtitle</t>
         </is>
       </c>
       <c r="C152" t="inlineStr"/>
@@ -4967,16 +5126,17 @@
       <c r="J152" t="inlineStr"/>
       <c r="K152" t="inlineStr"/>
       <c r="L152" t="inlineStr"/>
+      <c r="M152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>datacite:OtherTitle</t>
+          <t>datacite:TranslatedTitle</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>TranslatedTitle</t>
         </is>
       </c>
       <c r="C153" t="inlineStr"/>
@@ -4993,68 +5153,71 @@
       <c r="J153" t="inlineStr"/>
       <c r="K153" t="inlineStr"/>
       <c r="L153" t="inlineStr"/>
+      <c r="M153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>datacite:numberType</t>
+          <t>datacite:OtherTitleType</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>numberType</t>
-        </is>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>Type of the related item’s number, e.g., report number or article number.</t>
-        </is>
-      </c>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr"/>
       <c r="D154" t="inlineStr"/>
       <c r="E154" t="inlineStr"/>
-      <c r="F154" t="inlineStr"/>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>datacite:titleType</t>
+        </is>
+      </c>
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="inlineStr"/>
       <c r="I154" t="inlineStr"/>
       <c r="J154" t="inlineStr"/>
       <c r="K154" t="inlineStr"/>
       <c r="L154" t="inlineStr"/>
+      <c r="M154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>datacite:Article</t>
+          <t>datacite:numberType</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Article</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr"/>
+          <t>numberType</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Type of the related item’s number, e.g., report number or article number.</t>
+        </is>
+      </c>
       <c r="D155" t="inlineStr"/>
       <c r="E155" t="inlineStr"/>
-      <c r="F155" t="inlineStr">
-        <is>
-          <t>datacite:numberType</t>
-        </is>
-      </c>
+      <c r="F155" t="inlineStr"/>
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="inlineStr"/>
       <c r="I155" t="inlineStr"/>
       <c r="J155" t="inlineStr"/>
       <c r="K155" t="inlineStr"/>
       <c r="L155" t="inlineStr"/>
+      <c r="M155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>datacite:Chapter</t>
+          <t>datacite:Article</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Chapter</t>
+          <t>Article</t>
         </is>
       </c>
       <c r="C156" t="inlineStr"/>
@@ -5071,16 +5234,17 @@
       <c r="J156" t="inlineStr"/>
       <c r="K156" t="inlineStr"/>
       <c r="L156" t="inlineStr"/>
+      <c r="M156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>datacite:Report</t>
+          <t>datacite:Chapter</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Report</t>
+          <t>Chapter</t>
         </is>
       </c>
       <c r="C157" t="inlineStr"/>
@@ -5097,16 +5261,17 @@
       <c r="J157" t="inlineStr"/>
       <c r="K157" t="inlineStr"/>
       <c r="L157" t="inlineStr"/>
+      <c r="M157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>datacite:Other</t>
+          <t>datacite:Report</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Report</t>
         </is>
       </c>
       <c r="C158" t="inlineStr"/>
@@ -5123,68 +5288,71 @@
       <c r="J158" t="inlineStr"/>
       <c r="K158" t="inlineStr"/>
       <c r="L158" t="inlineStr"/>
+      <c r="M158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>datacite:funderIdentifierType</t>
+          <t>datacite:OtherNumberType</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>funderIdentifierType</t>
-        </is>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>The type of the funderIdentifier.</t>
-        </is>
-      </c>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr"/>
       <c r="D159" t="inlineStr"/>
       <c r="E159" t="inlineStr"/>
-      <c r="F159" t="inlineStr"/>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>datacite:numberType</t>
+        </is>
+      </c>
       <c r="G159" t="inlineStr"/>
       <c r="H159" t="inlineStr"/>
       <c r="I159" t="inlineStr"/>
       <c r="J159" t="inlineStr"/>
       <c r="K159" t="inlineStr"/>
       <c r="L159" t="inlineStr"/>
+      <c r="M159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>datacite:ISNI</t>
+          <t>datacite:funderIdentifierType</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>ISNI</t>
-        </is>
-      </c>
-      <c r="C160" t="inlineStr"/>
+          <t>funderIdentifierType</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>The type of the funderIdentifier.</t>
+        </is>
+      </c>
       <c r="D160" t="inlineStr"/>
       <c r="E160" t="inlineStr"/>
-      <c r="F160" t="inlineStr">
-        <is>
-          <t>datacite:funderIdentifierType</t>
-        </is>
-      </c>
+      <c r="F160" t="inlineStr"/>
       <c r="G160" t="inlineStr"/>
       <c r="H160" t="inlineStr"/>
       <c r="I160" t="inlineStr"/>
       <c r="J160" t="inlineStr"/>
       <c r="K160" t="inlineStr"/>
       <c r="L160" t="inlineStr"/>
+      <c r="M160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>datacite:GRID</t>
+          <t>datacite:ISNI</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>GRID</t>
+          <t>ISNI</t>
         </is>
       </c>
       <c r="C161" t="inlineStr"/>
@@ -5201,16 +5369,17 @@
       <c r="J161" t="inlineStr"/>
       <c r="K161" t="inlineStr"/>
       <c r="L161" t="inlineStr"/>
+      <c r="M161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>datacite:ROR</t>
+          <t>datacite:GRID</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>ROR</t>
+          <t>GRID</t>
         </is>
       </c>
       <c r="C162" t="inlineStr"/>
@@ -5227,16 +5396,17 @@
       <c r="J162" t="inlineStr"/>
       <c r="K162" t="inlineStr"/>
       <c r="L162" t="inlineStr"/>
+      <c r="M162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>datacite:CrossrefFunderID</t>
+          <t>datacite:ROR</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Crossref Funder ID</t>
+          <t>ROR</t>
         </is>
       </c>
       <c r="C163" t="inlineStr"/>
@@ -5253,16 +5423,17 @@
       <c r="J163" t="inlineStr"/>
       <c r="K163" t="inlineStr"/>
       <c r="L163" t="inlineStr"/>
+      <c r="M163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>datacite:OtherFunderIdentifierType</t>
+          <t>datacite:CrossrefFunderID</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Crossref Funder ID</t>
         </is>
       </c>
       <c r="C164" t="inlineStr"/>
@@ -5279,6 +5450,34 @@
       <c r="J164" t="inlineStr"/>
       <c r="K164" t="inlineStr"/>
       <c r="L164" t="inlineStr"/>
+      <c r="M164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>datacite:OtherFunderIdentifierType</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr"/>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>datacite:funderIdentifierType</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" t="inlineStr"/>
+      <c r="I165" t="inlineStr"/>
+      <c r="J165" t="inlineStr"/>
+      <c r="K165" t="inlineStr"/>
+      <c r="L165" t="inlineStr"/>
+      <c r="M165" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>